<commit_message>
Add the data converter.
</commit_message>
<xml_diff>
--- a/wwwroot/broker-report.xlsx
+++ b/wwwroot/broker-report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>GUARANTY TRUST BANK PLC ILUPEJU CASH CENTER</t>
   </si>
@@ -216,6 +216,45 @@
   </si>
   <si>
     <t>GUARANTY TRUST BANK PLC BOTH CASH CENTER</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>29,043</t>
+  </si>
+  <si>
+    <t>34,434</t>
+  </si>
+  <si>
+    <t>33,231</t>
+  </si>
+  <si>
+    <t>344,343</t>
+  </si>
+  <si>
+    <t>3,434</t>
+  </si>
+  <si>
+    <t>9,089</t>
+  </si>
+  <si>
+    <t>1,212</t>
+  </si>
+  <si>
+    <t>32,323</t>
+  </si>
+  <si>
+    <t>3,223</t>
+  </si>
+  <si>
+    <t>12,123</t>
   </si>
 </sst>
 </file>
@@ -285,17 +324,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A2:T30"/>
+  <dimension ref="A2:T41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="13.963663101196289" customWidth="1"/>
-    <col min="6" max="6" width="12.331873893737793" customWidth="1"/>
-    <col min="7" max="7" width="11.2382173538208" customWidth="1"/>
-    <col min="8" max="8" width="10.144560813903809" customWidth="1"/>
-    <col min="9" max="9" width="10.144560813903809" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1"/>
@@ -1377,6 +1416,303 @@
       </c>
       <c r="S30" s="0" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="34" ht="40" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="N36" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="O36" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="P36" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="N37" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="O37" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="P37" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="M38" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="N38" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="O38" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="P38" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="M39" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="N39" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="O39" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="P39" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P40" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P41" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1404,6 +1740,14 @@
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:T33"/>
+    <mergeCell ref="A34:T34"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>